<commit_message>
Finalizando o projeto e criando ranking
</commit_message>
<xml_diff>
--- a/dados.xlsx
+++ b/dados.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,25 +458,10 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>diego</t>
+          <t>17</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>tiao</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
         <v>25</v>
       </c>
     </row>

</xml_diff>